<commit_message>
EPBDS-9041 fix tests with DoubleRange
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/RangeContains.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/RangeContains.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EIS_Sources\OpenL\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA4E422-5D99-4E01-A888-E7ACB9B732E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CB542C-5452-450E-AB7B-9228180925D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RangeContains" sheetId="5" r:id="rId1"/>
@@ -195,15 +195,6 @@
     <t>= (BigDecimalValue) 1.1</t>
   </si>
   <si>
-    <t>= (float) 1.05</t>
-  </si>
-  <si>
-    <t>= (FloatValue) 1.05</t>
-  </si>
-  <si>
-    <t>= (Float) 1.05</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
@@ -229,6 +220,15 @@
   </si>
   <si>
     <t>= !contains($Value$IntRange, $Value)</t>
+  </si>
+  <si>
+    <t>= (float) 1.1</t>
+  </si>
+  <si>
+    <t>= (FloatValue) 1.1</t>
+  </si>
+  <si>
+    <t>= (Float) 1.1</t>
   </si>
 </sst>
 </file>
@@ -274,7 +274,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -318,9 +318,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -358,7 +358,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -464,7 +464,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -640,23 +640,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3FA0FE-50FB-4DE6-8A36-72A3D50C02EA}">
   <dimension ref="A4:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.59765625" customWidth="1"/>
-    <col min="3" max="3" width="20.06640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30.46484375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -670,7 +670,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +678,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -686,7 +686,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -700,7 +700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -714,7 +714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -728,7 +728,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -742,19 +742,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -766,7 +766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -780,7 +780,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -794,7 +794,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>2</v>
       </c>
@@ -808,7 +808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -822,19 +822,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -846,7 +846,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -860,7 +860,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -872,7 +872,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -886,7 +886,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>20</v>
       </c>
@@ -900,7 +900,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>21</v>
       </c>
@@ -914,7 +914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>22</v>
       </c>
@@ -928,19 +928,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>24</v>
       </c>
@@ -952,7 +952,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>25</v>
       </c>
@@ -966,7 +966,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>26</v>
       </c>
@@ -978,88 +978,88 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1076,20 +1076,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26F9E5E-F254-40A0-B439-21CF1C354CEE}">
   <dimension ref="A5:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.53125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.53125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="39.265625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="44.06640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.53125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="39.21875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="44.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
@@ -1101,7 +1101,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1119,7 +1119,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1147,7 +1147,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1165,7 +1165,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1183,7 +1183,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1201,7 +1201,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1219,15 +1219,15 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>30</v>
@@ -1237,7 +1237,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>30</v>
@@ -1255,7 +1255,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1273,7 +1273,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1291,7 +1291,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1309,7 +1309,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1327,15 +1327,15 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>30</v>
@@ -1345,7 +1345,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>30</v>
@@ -1363,7 +1363,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
@@ -1381,7 +1381,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>18</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>30</v>
@@ -1399,7 +1399,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
@@ -1417,7 +1417,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
@@ -1435,7 +1435,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
@@ -1453,7 +1453,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
@@ -1471,15 +1471,15 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>30</v>
@@ -1489,7 +1489,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>24</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>52</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>30</v>
@@ -1507,7 +1507,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>25</v>
       </c>
@@ -1525,7 +1525,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>54</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>30</v>
@@ -1543,23 +1543,23 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1569,97 +1569,97 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>

</xml_diff>